<commit_message>
SB.Common TemplateReportObjectExporter logic added
</commit_message>
<xml_diff>
--- a/NUnit Tests/SB.Report.Test/Logics/ExcelTemplate/Reports/CustomExcelTemplateReport.xlsx
+++ b/NUnit Tests/SB.Report.Test/Logics/ExcelTemplate/Reports/CustomExcelTemplateReport.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mansur\source\repos\SBFramework\NUnit Tests\SB.Report.Test\Logics\ExcelTemplate\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bunyod\Desktop\Projects\SBFramework\NUnit Tests\SB.Report.Test\Logics\ExcelTemplate\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E1CAE7-CA17-4E9F-A772-7601D51756B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$3:$K$3</definedName>
-    <definedName name="header">Лист1!$A$1:$K$3</definedName>
-    <definedName name="row">Лист1!$A$4:$K$4</definedName>
+    <definedName name="Header">Лист1!$A$1:$K$3</definedName>
+    <definedName name="Rows">Лист1!$A$4:$K$4</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -105,7 +104,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_р_._-;\-* #,##0_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
@@ -297,23 +296,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -349,23 +331,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -541,11 +506,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,7 +560,7 @@
       <c r="I2" s="15"/>
       <c r="J2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>

</xml_diff>